<commit_message>
db data insertion into excel
</commit_message>
<xml_diff>
--- a/src/databaseSheet.xlsx
+++ b/src/databaseSheet.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="employee" r:id="rId2" sheetId="1" state="visible"/>
     <sheet name="result" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="dbdata" r:id="rId4" sheetId="3" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -44,10 +45,28 @@
     <t xml:space="preserve">pavan@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Excel record value is raesh  but data base record value is  rakesh</t>
+    <t xml:space="preserve">Error : Excel record value is raesh  but data base record value is  rakesh</t>
   </si>
   <si>
     <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t>rakesh</t>
+  </si>
+  <si>
+    <t>rakesh@gmail.com</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>pavan</t>
+  </si>
+  <si>
+    <t>pavan@gmail.com</t>
+  </si>
+  <si>
+    <t>18000</t>
   </si>
   <si>
     <t>Error : Excel record value is raesh  but data base record value is  rakesh</t>
@@ -169,7 +188,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -235,8 +254,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -247,12 +266,64 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="30.56" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="27.38" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="19.72" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with realative file path
</commit_message>
<xml_diff>
--- a/src/databaseSheet.xlsx
+++ b/src/databaseSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="employee" r:id="rId2" sheetId="1" state="visible"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -30,9 +30,6 @@
     <t xml:space="preserve">email</t>
   </si>
   <si>
-    <t xml:space="preserve">salary</t>
-  </si>
-  <si>
     <t xml:space="preserve">raesh</t>
   </si>
   <si>
@@ -51,22 +48,19 @@
     <t xml:space="preserve">true</t>
   </si>
   <si>
+    <t xml:space="preserve">rakesh</t>
+  </si>
+  <si>
     <t>rakesh</t>
   </si>
   <si>
     <t>rakesh@gmail.com</t>
   </si>
   <si>
-    <t>20000</t>
-  </si>
-  <si>
     <t>pavan</t>
   </si>
   <si>
     <t>pavan@gmail.com</t>
-  </si>
-  <si>
-    <t>18000</t>
   </si>
   <si>
     <t>Error : Excel record value is raesh  but data base record value is  rakesh</t>
@@ -185,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E12" activeCellId="0" pane="topLeft" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -206,30 +200,21 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>20000</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>18000</v>
       </c>
     </row>
   </sheetData>
@@ -255,7 +240,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
+      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -266,12 +251,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -290,10 +275,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="1:1048576"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -311,19 +296,13 @@
       <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>